<commit_message>
re-upload bug-report to fix formatting
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariannajoe/UBC Courses/2023W/2023W2/CPSC427/Project/M1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF850E62-EE49-804B-80C3-F0BAA353EF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2D73D-5920-214B-97A6-A4E138D612F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6600" yWindow="1140" windowWidth="19660" windowHeight="16540" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
@@ -274,16 +274,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,7 +623,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E9"/>
+      <selection activeCell="G10" sqref="G10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,199 +673,217 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="12">
         <v>45337</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="9" t="s">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+    <row r="6" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="11">
         <v>2</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="12">
         <v>45335</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="9" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>3</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>45338</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="9" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="I10:I12"/>
@@ -875,24 +893,6 @@
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating readme, bug report and test plan docs
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariannajoe/UBC Courses/2023W/2023W2/CPSC427/Project/M1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracychow/Dropbox/My Mac (Tracy’s MacBook Pro)/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2D73D-5920-214B-97A6-A4E138D612F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D87C96-91BE-A949-B3FC-4798742D1E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="1140" windowWidth="19660" windowHeight="16540" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="bugs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>#</t>
   </si>
@@ -178,6 +178,78 @@
   </si>
   <si>
     <t>Press C again after a few seconds to observe changes in player position.</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Game crashes when running in debug (works in release)</t>
+  </si>
+  <si>
+    <t>Game should start and window should render</t>
+  </si>
+  <si>
+    <t>Nothing renders and there’s an assert failure</t>
+  </si>
+  <si>
+    <t>Run game with configuration set to Debug</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Miss SFX sometimes does not play if too many happen</t>
+  </si>
+  <si>
+    <t>Every time a player presses a key where there is no collision, a miss SFX should play</t>
+  </si>
+  <si>
+    <t>If player misses many notes, then no miss SFX will play after about, maybe due to SDL channel limitations</t>
+  </si>
+  <si>
+    <t>Spam all DFJK keys rapidly, and notice that there are intervals where no miss SFX will play</t>
+  </si>
+  <si>
+    <t>Walking animation stops when 2 keys are pressed down at the same time</t>
+  </si>
+  <si>
+    <t>Animation continues as usual</t>
+  </si>
+  <si>
+    <t>Walking animation is paused and sometimes resumes jerkily</t>
+  </si>
+  <si>
+    <t>Hold down a direction key (WASD)</t>
+  </si>
+  <si>
+    <t>While holding down that key press and hold another direction key</t>
+  </si>
+  <si>
+    <t>Single key press can trigger two collisions at same time</t>
+  </si>
+  <si>
+    <t>When there are two notes colliding with the same judgment line, only the lowest one should be removed on player input.</t>
+  </si>
+  <si>
+    <t>All notes colliding with judgment line at the time of player input will be removed.</t>
+  </si>
+  <si>
+    <t>Wait for opportunity where there are two notes close together in the same lane. Time the appropriate DFJK input when both notes are colliding with the judgment line.</t>
+  </si>
+  <si>
+    <t>After entering battle by collision, when the battle over pop up appears, it renders behind the notes</t>
+  </si>
+  <si>
+    <t>Pop up should render over all on-screen entities</t>
+  </si>
+  <si>
+    <t>Pop up renders behind falling notes and sprite portraits in battle screen</t>
+  </si>
+  <si>
+    <t>Enter a battle by collision and either trigger or wait for battle end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most easily reproduceable in enemy1 (second battle) due to notes in quick succession. </t>
   </si>
 </sst>
 </file>
@@ -249,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -260,7 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -270,19 +341,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,252 +697,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="1" max="4" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
     <col min="7" max="7" width="27.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="26" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="32.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+    <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>45337</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="E4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="7" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="8">
         <v>45335</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="7" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>3</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>45338</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
+      <c r="E10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="7" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="7" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+    <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="13">
+        <v>45351</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>45353</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>6</v>
+      </c>
+      <c r="B15" s="12">
+        <v>45354</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>7</v>
+      </c>
+      <c r="B17" s="12">
+        <v>45353</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>8</v>
+      </c>
+      <c r="B19" s="13">
+        <v>45355</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="45">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="A4:A6"/>
@@ -879,20 +1157,6 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating test plan and bug list
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracychow/Dropbox/My Mac (Tracy’s MacBook Pro)/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracychow/Documents/School/2023W/CPSC 427/Team-2-Harmonic-Hustle/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D87C96-91BE-A949-B3FC-4798742D1E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7727BB59-6691-BE43-BFD8-10300A4B2E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{A93FC866-1E7B-484F-97FF-E98B7C804DE3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Sherry</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>When resizing the window, the screen boundry gets messed up and the scale of characters seems to change with the window size</t>
   </si>
   <si>
@@ -250,13 +247,140 @@
   </si>
   <si>
     <t xml:space="preserve">Most easily reproduceable in enemy1 (second battle) due to notes in quick succession. </t>
+  </si>
+  <si>
+    <t>Arianna</t>
+  </si>
+  <si>
+    <t>Resolved
+(Collect all collisions first, then remove only the lowest note in each lane)</t>
+  </si>
+  <si>
+    <t>Crash on C key in battle scene.</t>
+  </si>
+  <si>
+    <t>Game should never crash during battle scene on any key press.</t>
+  </si>
+  <si>
+    <t>Game sometimes crashes during battle on pressing C key.</t>
+  </si>
+  <si>
+    <t>Resolved
+Added more guards in code. May have been due to key presses being a callback (?), and entities being removed unexpectedly.</t>
+  </si>
+  <si>
+    <t>When pressing C when 3 or more notes are on screen (now with particles), game will crash. *Seems to be related to deleting generators in render_system.cpp. Commenting out prevents crashes but will cause memory leak.</t>
+  </si>
+  <si>
+    <t>Resolved
+(Dummy spark-particle entities were not being removed from registry after effect expired)</t>
+  </si>
+  <si>
+    <t>Game lags when many notes are on screen</t>
+  </si>
+  <si>
+    <t>Game should run smoothly even when many notes are on screen.</t>
+  </si>
+  <si>
+    <t>Game lags in battle scene when many notes are on screen.</t>
+  </si>
+  <si>
+    <t>Most noticeable in the middle of level 2. Simply watch the FPS counter drop over time</t>
+  </si>
+  <si>
+    <t>Tiny particle(s) in top left corner</t>
+  </si>
+  <si>
+    <t>No particles should appear in top left corner in battle scene</t>
+  </si>
+  <si>
+    <t>There are tiny particles with unchanging values in the top left corner of battle scene</t>
+  </si>
+  <si>
+    <t>Enter battle scene</t>
+  </si>
+  <si>
+    <t>Resolved
+(Unused particle data in memory had default colour of 1.f; set it to 0.f instead)</t>
+  </si>
+  <si>
+    <t>FPS may drop due to text-rendering taking particularly long (relative to other game loop steps).</t>
+  </si>
+  <si>
+    <t>FPS should remain above 60 at all times</t>
+  </si>
+  <si>
+    <t>FPS drops proportionally to the amount of text on screen</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experienced on Mac M2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, but not Windows PC.
+Play game, watch FPS counter. Uncomment profiling code in render_system.cpp to see runtimes measured in ms.
+Not a huge problem right now since our text is limited, and lowest FPS is during static moments (battle-over screen). But it will be a bottleneck if we add more in battle scene especially</t>
+    </r>
+  </si>
+  <si>
+    <t>Character portrait scale discrepancy</t>
+  </si>
+  <si>
+    <t>Scale of assets to be the same</t>
+  </si>
+  <si>
+    <t>Scale of assets is different and may be bigger or smaller depending on the screen</t>
+  </si>
+  <si>
+    <t>Open game, go to cutscene on 2 different resolution monitors</t>
+  </si>
+  <si>
+    <t>Game not restarting as expected after colliding with high level enemy</t>
+  </si>
+  <si>
+    <t>New game should be started after clicking "New game" in start screen</t>
+  </si>
+  <si>
+    <t>Player enters the game over screen after colliding with high level enemy. Pressing SPACE key takes player back to the start screen. Clicking the "New game" button starts a new game</t>
+  </si>
+  <si>
+    <t>Player is taken directly back to game over screen. New game doesn't start</t>
+  </si>
+  <si>
+    <t>Game not loading properly after saving a finished game</t>
+  </si>
+  <si>
+    <t>Game should start a new game if saved game is finished</t>
+  </si>
+  <si>
+    <t>Nothing gets rendered on screen after clicking "Load" on start screen</t>
+  </si>
+  <si>
+    <t>Have a saved game where player level = 4 and gameIsOver = true. Launch game and click "Load" in start screen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +418,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -321,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,6 +472,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -350,18 +493,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -697,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B0CA0-DDFC-4447-897A-42A4E259D7BB}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I12"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -716,7 +854,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -753,361 +891,581 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="12">
         <v>45337</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12">
+        <v>45335</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6" t="s">
+      <c r="G7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>3</v>
+      </c>
+      <c r="B10" s="12">
+        <v>45338</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8">
-        <v>45335</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8">
-        <v>45338</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="G10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="6" t="s">
+    <row r="12" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>4</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="8">
         <v>45351</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="8">
         <v>45353</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>6</v>
+      </c>
+      <c r="B15" s="15">
+        <v>45354</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>6</v>
-      </c>
-      <c r="B15" s="12">
-        <v>45354</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="I15" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="1" t="s">
+    <row r="17" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>7</v>
+      </c>
+      <c r="B17" s="15">
+        <v>45353</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11">
-        <v>7</v>
-      </c>
-      <c r="B17" s="12">
-        <v>45353</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11" t="s">
+      <c r="H17" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="I17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="J17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>8</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="8">
         <v>45355</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>69</v>
+    </row>
+    <row r="20" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>9</v>
+      </c>
+      <c r="B20" s="8">
+        <v>45370</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>10</v>
+      </c>
+      <c r="B21" s="8">
+        <v>45375</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8">
+        <v>45375</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>12</v>
+      </c>
+      <c r="B23" s="16">
+        <v>45377</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>13</v>
+      </c>
+      <c r="B24" s="8">
+        <v>45377</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>14</v>
+      </c>
+      <c r="B25" s="8">
+        <v>45375</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>15</v>
+      </c>
+      <c r="B26" s="8">
+        <v>45377</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>